<commit_message>
feat: another anova, finally
</commit_message>
<xml_diff>
--- a/data/raw/AnswersDepurated.xlsx
+++ b/data/raw/AnswersDepurated.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kennet\OneDrive - Universidad Icesi (@icesi.edu.co)\Universidad\Quinto semestre\Inferencia estadística\free-to-play-r\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\College\22-2\IE\code\free-to-play-r\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0AC357-D303-4F70-892E-651222C738F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122CC24F-C042-4511-8B99-01451E2F3AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas de formulario 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Respuestas de formulario 1'!$A$1:$N$130</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="22">
   <si>
     <t>RPG/Juegos de rol</t>
   </si>
@@ -40,16 +43,10 @@
     <t>Shooters/Battle Royale/Juegos de disparos</t>
   </si>
   <si>
-    <t>Carreras/Conduccion</t>
-  </si>
-  <si>
     <t>Gacha/Juegos con lootboxes</t>
   </si>
   <si>
     <t>Puzzles</t>
-  </si>
-  <si>
-    <t>Deportes</t>
   </si>
   <si>
     <t>juegaVideojuegos</t>
@@ -411,66 +408,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M51" sqref="M51"/>
+      <selection pane="bottomLeft" activeCell="L138" sqref="L138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="18.85546875" customWidth="1"/>
+    <col min="1" max="15" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -498,14 +495,14 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
+      <c r="J2" s="3">
+        <v>2</v>
       </c>
       <c r="K2" s="1">
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M2" s="2">
         <v>5</v>
@@ -514,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -549,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M3" s="2">
         <v>7</v>
@@ -558,7 +555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -587,13 +584,13 @@
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M4" s="2">
         <v>7</v>
@@ -602,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -631,13 +628,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M5" s="2">
         <v>7</v>
@@ -646,7 +643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -681,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M6" s="2">
         <v>10</v>
@@ -690,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -719,13 +716,13 @@
         <v>1</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M7" s="2">
         <v>10</v>
@@ -734,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -763,13 +760,13 @@
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M8" s="2">
         <v>8</v>
@@ -778,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -807,13 +804,13 @@
         <v>1</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1">
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M9" s="2">
         <v>4</v>
@@ -822,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -851,13 +848,13 @@
         <v>1</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M10" s="2">
         <v>7</v>
@@ -866,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -894,14 +891,14 @@
       <c r="I11" s="2">
         <v>1</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>5</v>
+      <c r="J11" s="3">
+        <v>2</v>
       </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M11" s="2">
         <v>3</v>
@@ -910,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -945,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M12" s="2">
         <v>3</v>
@@ -954,7 +951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -989,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M13" s="2">
         <v>2</v>
@@ -998,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
@@ -1042,7 +1039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -1077,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M15" s="2">
         <v>6</v>
@@ -1086,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
@@ -1115,13 +1112,13 @@
         <v>1</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M16" s="2">
         <v>2</v>
@@ -1130,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -1159,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M17" s="2">
         <v>10</v>
@@ -1174,7 +1171,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M18" s="2">
         <v>6</v>
@@ -1218,7 +1215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>1</v>
       </c>
@@ -1247,13 +1244,13 @@
         <v>0</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K19" s="1">
         <v>1</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M19" s="2">
         <v>9</v>
@@ -1262,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>1</v>
       </c>
@@ -1291,13 +1288,13 @@
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M20" s="2">
         <v>4</v>
@@ -1306,7 +1303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -1334,14 +1331,14 @@
       <c r="I21" s="2">
         <v>1</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>5</v>
+      <c r="J21" s="3">
+        <v>2</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M21" s="2">
         <v>9</v>
@@ -1350,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1385,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M22" s="2">
         <v>3</v>
@@ -1394,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -1422,14 +1419,14 @@
       <c r="I23" s="2">
         <v>1</v>
       </c>
-      <c r="J23" s="3" t="s">
-        <v>5</v>
+      <c r="J23" s="3">
+        <v>2</v>
       </c>
       <c r="K23" s="1">
         <v>0</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M23" s="2">
         <v>9</v>
@@ -1438,7 +1435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -1473,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M24" s="2">
         <v>5</v>
@@ -1482,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -1517,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M25" s="2">
         <v>0</v>
@@ -1526,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -1561,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M26" s="2">
         <v>2</v>
@@ -1570,7 +1567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>1</v>
       </c>
@@ -1599,13 +1596,13 @@
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K27" s="1">
         <v>1</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M27" s="2">
         <v>7</v>
@@ -1614,7 +1611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="53.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>1</v>
       </c>
@@ -1642,14 +1639,14 @@
       <c r="I28" s="2">
         <v>0</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>2</v>
+      <c r="J28" s="1">
+        <v>1</v>
       </c>
       <c r="K28" s="1">
         <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M28" s="2">
         <v>1</v>
@@ -1658,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="53.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>1</v>
       </c>
@@ -1693,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M29" s="2">
         <v>1</v>
@@ -1702,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>1</v>
       </c>
@@ -1731,13 +1728,13 @@
         <v>1</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K30" s="1">
         <v>1</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M30" s="2">
         <v>8</v>
@@ -1746,7 +1743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>1</v>
       </c>
@@ -1781,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M31" s="2">
         <v>1</v>
@@ -1790,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>1</v>
       </c>
@@ -1819,13 +1816,13 @@
         <v>0</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K32" s="1">
         <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M32" s="2">
         <v>6</v>
@@ -1834,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>1</v>
       </c>
@@ -1869,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M33" s="2">
         <v>3</v>
@@ -1878,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>1</v>
       </c>
@@ -1913,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M34" s="2">
         <v>1</v>
@@ -1922,7 +1919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>1</v>
       </c>
@@ -1951,13 +1948,13 @@
         <v>1</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K35" s="1">
         <v>1</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M35" s="2">
         <v>3</v>
@@ -1966,7 +1963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -1995,13 +1992,13 @@
         <v>1</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K36" s="1">
         <v>0</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M36" s="2">
         <v>10</v>
@@ -2010,7 +2007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="40.200000000000003" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>1</v>
       </c>
@@ -2045,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M37" s="2">
         <v>10</v>
@@ -2054,7 +2051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="13.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>1</v>
       </c>
@@ -2089,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M38" s="2">
         <v>4</v>
@@ -2098,94 +2095,108 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="130" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:14" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="13.2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="5:5" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="5:5" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E130" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N130" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Gacha/Juegos con lootboxes"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N130">
     <sortCondition descending="1" ref="D1:D130"/>
   </sortState>

</xml_diff>